<commit_message>
Dodano dodawanie recept dla pacjenta
</commit_message>
<xml_diff>
--- a/drugs.xlsx
+++ b/drugs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E201"/>
+  <dimension ref="A1:E210"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5060,6 +5060,123 @@
         </is>
       </c>
     </row>
+    <row r="202">
+      <c r="A202" t="n">
+        <v>201</v>
+      </c>
+      <c r="B202" t="inlineStr"/>
+      <c r="C202" t="inlineStr"/>
+      <c r="D202" t="inlineStr"/>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>2025-06-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="n">
+        <v>202</v>
+      </c>
+      <c r="B203" t="inlineStr"/>
+      <c r="C203" t="inlineStr"/>
+      <c r="D203" t="inlineStr"/>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>2025-06-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="n">
+        <v>203</v>
+      </c>
+      <c r="B204" t="inlineStr"/>
+      <c r="C204" t="inlineStr"/>
+      <c r="D204" t="inlineStr"/>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>2025-06-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="n">
+        <v>204</v>
+      </c>
+      <c r="B205" t="inlineStr"/>
+      <c r="C205" t="inlineStr"/>
+      <c r="D205" t="inlineStr"/>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>2025-06-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="n">
+        <v>205</v>
+      </c>
+      <c r="B206" t="inlineStr"/>
+      <c r="C206" t="inlineStr"/>
+      <c r="D206" t="inlineStr"/>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>2025-06-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="n">
+        <v>206</v>
+      </c>
+      <c r="B207" t="inlineStr"/>
+      <c r="C207" t="inlineStr"/>
+      <c r="D207" t="inlineStr"/>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>2025-06-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="n">
+        <v>207</v>
+      </c>
+      <c r="B208" t="inlineStr"/>
+      <c r="C208" t="inlineStr"/>
+      <c r="D208" t="inlineStr"/>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>2025-06-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="n">
+        <v>208</v>
+      </c>
+      <c r="B209" t="inlineStr"/>
+      <c r="C209" t="inlineStr"/>
+      <c r="D209" t="inlineStr"/>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>2025-06-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="n">
+        <v>209</v>
+      </c>
+      <c r="B210" t="inlineStr"/>
+      <c r="C210" t="inlineStr"/>
+      <c r="D210" t="inlineStr"/>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>2025-06-08</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Rozdzielono zakup na receptę i bez recepty
</commit_message>
<xml_diff>
--- a/drugs.xlsx
+++ b/drugs.xlsx
@@ -498,7 +498,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>430</v>
+        <v>421</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -751,7 +751,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -820,7 +820,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>

</xml_diff>